<commit_message>
excel sheets & tets data
</commit_message>
<xml_diff>
--- a/data/results.xlsx
+++ b/data/results.xlsx
@@ -8392,11 +8392,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="437107696"/>
-        <c:axId val="437104952"/>
+        <c:axId val="381320784"/>
+        <c:axId val="381317256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="437107696"/>
+        <c:axId val="381320784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8453,12 +8453,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437104952"/>
+        <c:crossAx val="381317256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="437104952"/>
+        <c:axId val="381317256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8515,7 +8515,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437107696"/>
+        <c:crossAx val="381320784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8603,7 +8603,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> &amp; 3de Kwantielen</a:t>
+              <a:t> &amp; 3de Kwartielen</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -8641,13 +8641,26 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1584503937007874"/>
+          <c:y val="0.14275555555555558"/>
+          <c:w val="0.78375419072615926"/>
+          <c:h val="0.5511493729950423"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>1ste kwartiel</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -8657,7 +8670,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -8822,6 +8835,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>2de kwartiel</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -8830,8 +8846,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="square"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -9001,11 +9017,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="431346888"/>
-        <c:axId val="431338264"/>
+        <c:axId val="381315688"/>
+        <c:axId val="381309024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="431346888"/>
+        <c:axId val="381315688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9025,6 +9041,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t># elementen in steekproef</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -9062,12 +9134,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="431338264"/>
+        <c:crossAx val="381309024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="431338264"/>
+        <c:axId val="381309024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9087,6 +9159,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Gemeten</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> hoogte (cm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -9124,7 +9257,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="431346888"/>
+        <c:crossAx val="381315688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9138,6 +9271,14 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -9240,11 +9381,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Varientie</a:t>
+              <a:t>Variantie</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> en Inter Kwantiele afstanden</a:t>
+              <a:t> en Inter Kwartiele afstanden</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -9282,13 +9423,26 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15290372703412072"/>
+          <c:y val="0.1723851851851852"/>
+          <c:w val="0.78930085739282585"/>
+          <c:h val="0.51781673957421992"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>IQR</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -9297,8 +9451,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="square"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -9448,6 +9602,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Variantie</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -9457,7 +9614,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -9612,11 +9769,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="433263992"/>
-        <c:axId val="433262816"/>
+        <c:axId val="381319216"/>
+        <c:axId val="381309416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="433263992"/>
+        <c:axId val="381319216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9636,6 +9793,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>#</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> elementen in steekproef</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -9673,12 +9891,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="433262816"/>
+        <c:crossAx val="381309416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="433262816"/>
+        <c:axId val="381309416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9698,6 +9916,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Variantie</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> en IQR (cm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -9735,7 +10014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="433263992"/>
+        <c:crossAx val="381319216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11518,16 +11797,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>44</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>628649</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>109536</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>49</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>157161</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11548,16 +11827,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>52</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>109536</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>55</xdr:col>
-      <xdr:colOff>1019175</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>1104899</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>157161</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11848,8 +12127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR4" workbookViewId="0">
-      <selection activeCell="AZ30" sqref="AZ30"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="BF5" sqref="BF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>